<commit_message>
updated iris.xlsx with polynomial kernel results
Description: Updated iris.xlsx with polynomial kernel results

Commit: Add

TaskNumber:#0
</commit_message>
<xml_diff>
--- a/results/knn-ald_iris/Iris.xlsx
+++ b/results/knn-ald_iris/Iris.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\MLTool_matlab\results\knn-ald_iris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F19272B-2FBD-4273-AD52-4798576CC2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64F444C-BB88-4F7B-AA51-CC53B775891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="54">
   <si>
     <t>4 attributes</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>gamma</t>
+  </si>
+  <si>
+    <t>0.0078</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.8</t>
   </si>
 </sst>
 </file>
@@ -305,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,10 +352,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,28 +720,28 @@
       <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="14">
-        <v>2</v>
-      </c>
-      <c r="H4" s="14">
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
         <v>5</v>
       </c>
-      <c r="I4" s="14">
-        <v>2</v>
-      </c>
-      <c r="J4" s="14">
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
         <v>2</v>
       </c>
       <c r="K4" s="2">
@@ -740,28 +751,28 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="6"/>
-      <c r="C5" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="1">
         <v>6</v>
       </c>
-      <c r="I5" s="14">
-        <v>2</v>
-      </c>
-      <c r="J5" s="14">
+      <c r="I5" s="1">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1">
         <v>2</v>
       </c>
       <c r="K5" s="2">
@@ -774,28 +785,28 @@
       <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="14" t="s">
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="14">
-        <v>4</v>
-      </c>
-      <c r="H6" s="14">
-        <v>4</v>
-      </c>
-      <c r="I6" s="14">
-        <v>1</v>
-      </c>
-      <c r="J6" s="14">
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
         <v>1</v>
       </c>
       <c r="K6" s="2">
@@ -806,28 +817,28 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="14">
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
         <v>100</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="14">
-        <v>2</v>
-      </c>
-      <c r="G7" s="14">
-        <v>4</v>
-      </c>
-      <c r="H7" s="14">
-        <v>4</v>
-      </c>
-      <c r="I7" s="14">
-        <v>1</v>
-      </c>
-      <c r="J7" s="14">
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
         <v>1</v>
       </c>
       <c r="K7" s="2">
@@ -838,14 +849,6 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
       <c r="K8" s="3"/>
       <c r="L8" s="1"/>
     </row>
@@ -856,28 +859,28 @@
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="14" t="s">
+      <c r="E9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="1">
         <v>5</v>
       </c>
-      <c r="I9" s="14">
-        <v>1</v>
-      </c>
-      <c r="J9" s="14">
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
         <v>2</v>
       </c>
       <c r="K9" s="2">
@@ -888,28 +891,28 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="14" t="s">
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14">
-        <v>4</v>
-      </c>
-      <c r="H10" s="14">
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1">
         <v>8</v>
       </c>
-      <c r="I10" s="14">
-        <v>2</v>
-      </c>
-      <c r="J10" s="14">
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1">
         <v>3</v>
       </c>
       <c r="K10" s="2">
@@ -922,28 +925,28 @@
       <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="1">
         <v>9</v>
       </c>
-      <c r="I11" s="14">
-        <v>1</v>
-      </c>
-      <c r="J11" s="14">
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
         <v>4</v>
       </c>
       <c r="K11" s="2">
@@ -954,28 +957,28 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="14" t="s">
+      <c r="E12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="1">
         <v>11</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="1">
         <v>3</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="1">
         <v>4</v>
       </c>
       <c r="K12" s="2">
@@ -986,14 +989,14 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
       <c r="K13" s="2"/>
       <c r="L13" s="1"/>
     </row>
@@ -1004,28 +1007,28 @@
       <c r="B14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="14" t="s">
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="14">
-        <v>4</v>
-      </c>
-      <c r="I14" s="14">
-        <v>2</v>
-      </c>
-      <c r="J14" s="14">
+      <c r="H14" s="1">
+        <v>4</v>
+      </c>
+      <c r="I14" s="1">
+        <v>2</v>
+      </c>
+      <c r="J14" s="1">
         <v>1</v>
       </c>
       <c r="K14" s="2">
@@ -1036,28 +1039,28 @@
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="14" t="s">
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="14">
-        <v>1</v>
-      </c>
-      <c r="G15" s="14" t="s">
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="14">
-        <v>4</v>
-      </c>
-      <c r="I15" s="14">
-        <v>1</v>
-      </c>
-      <c r="J15" s="14">
+      <c r="H15" s="1">
+        <v>4</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1">
         <v>1</v>
       </c>
       <c r="K15" s="2">
@@ -1070,28 +1073,28 @@
       <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="14" t="s">
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="14">
-        <v>4</v>
-      </c>
-      <c r="H16" s="14">
+      <c r="G16" s="1">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1">
         <v>7</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="1">
         <v>3</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="1">
         <v>2</v>
       </c>
       <c r="K16" s="2">
@@ -1102,28 +1105,28 @@
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="14" t="s">
+      <c r="C17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="14">
-        <v>1</v>
-      </c>
-      <c r="G17" s="14" t="s">
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="14">
-        <v>4</v>
-      </c>
-      <c r="I17" s="14">
-        <v>1</v>
-      </c>
-      <c r="J17" s="14">
+      <c r="H17" s="1">
+        <v>4</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1">
         <v>1</v>
       </c>
       <c r="K17" s="2">
@@ -1134,14 +1137,13 @@
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
       <c r="K18" s="2"/>
       <c r="L18" s="1"/>
     </row>
@@ -1152,28 +1154,28 @@
       <c r="B19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="14" t="s">
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="14">
-        <v>4</v>
-      </c>
-      <c r="H19" s="14">
+      <c r="G19" s="1">
+        <v>4</v>
+      </c>
+      <c r="H19" s="1">
         <v>5</v>
       </c>
-      <c r="I19" s="14">
-        <v>2</v>
-      </c>
-      <c r="J19" s="14">
+      <c r="I19" s="1">
+        <v>2</v>
+      </c>
+      <c r="J19" s="1">
         <v>2</v>
       </c>
       <c r="K19" s="2">
@@ -1184,28 +1186,28 @@
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="14" t="s">
+      <c r="C20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="14" t="s">
+      <c r="E20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="14">
-        <v>2</v>
-      </c>
-      <c r="H20" s="14">
+      <c r="G20" s="1">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1">
         <v>10</v>
       </c>
-      <c r="I20" s="14">
-        <v>2</v>
-      </c>
-      <c r="J20" s="14">
+      <c r="I20" s="1">
+        <v>2</v>
+      </c>
+      <c r="J20" s="1">
         <v>4</v>
       </c>
       <c r="K20" s="2">
@@ -1218,28 +1220,28 @@
       <c r="B21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="14" t="s">
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="1">
         <v>100</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="1">
         <v>5</v>
       </c>
-      <c r="I21" s="14">
-        <v>2</v>
-      </c>
-      <c r="J21" s="14">
+      <c r="I21" s="1">
+        <v>2</v>
+      </c>
+      <c r="J21" s="1">
         <v>2</v>
       </c>
       <c r="K21" s="2">
@@ -1331,28 +1333,28 @@
       <c r="B25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="14" t="s">
+      <c r="C25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="14">
-        <v>4</v>
-      </c>
-      <c r="H25" s="14">
+      <c r="G25" s="1">
+        <v>4</v>
+      </c>
+      <c r="H25" s="1">
         <v>6</v>
       </c>
-      <c r="I25" s="14">
-        <v>2</v>
-      </c>
-      <c r="J25" s="14">
+      <c r="I25" s="1">
+        <v>2</v>
+      </c>
+      <c r="J25" s="1">
         <v>2</v>
       </c>
       <c r="K25" s="2">
@@ -1362,28 +1364,28 @@
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="14" t="s">
+      <c r="C26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="14">
-        <v>4</v>
-      </c>
-      <c r="H26" s="14">
-        <v>4</v>
-      </c>
-      <c r="I26" s="14">
-        <v>1</v>
-      </c>
-      <c r="J26" s="14">
+      <c r="G26" s="1">
+        <v>4</v>
+      </c>
+      <c r="H26" s="1">
+        <v>4</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1">
         <v>1</v>
       </c>
       <c r="K26" s="2">
@@ -1396,28 +1398,28 @@
       <c r="B27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="14" t="s">
+      <c r="C27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G27" s="14">
-        <v>4</v>
-      </c>
-      <c r="H27" s="14">
-        <v>4</v>
-      </c>
-      <c r="I27" s="14">
-        <v>2</v>
-      </c>
-      <c r="J27" s="14">
+      <c r="G27" s="1">
+        <v>4</v>
+      </c>
+      <c r="H27" s="1">
+        <v>4</v>
+      </c>
+      <c r="I27" s="1">
+        <v>2</v>
+      </c>
+      <c r="J27" s="1">
         <v>1</v>
       </c>
       <c r="K27" s="2">
@@ -1428,28 +1430,28 @@
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="14" t="s">
+      <c r="C28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" s="14" t="s">
+      <c r="E28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="14">
-        <v>4</v>
-      </c>
-      <c r="H28" s="14">
-        <v>4</v>
-      </c>
-      <c r="I28" s="14">
-        <v>1</v>
-      </c>
-      <c r="J28" s="14">
+      <c r="G28" s="1">
+        <v>4</v>
+      </c>
+      <c r="H28" s="1">
+        <v>4</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1">
         <v>2</v>
       </c>
       <c r="K28" s="2">
@@ -1460,14 +1462,6 @@
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1477,28 +1471,28 @@
       <c r="B30" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="14" t="s">
+      <c r="C30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="1">
         <v>8</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="1">
         <v>8</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I30" s="1">
         <v>3</v>
       </c>
-      <c r="J30" s="14">
+      <c r="J30" s="1">
         <v>2</v>
       </c>
       <c r="K30" s="2">
@@ -1508,28 +1502,28 @@
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="14" t="s">
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="1">
         <v>8</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="1">
         <v>10</v>
       </c>
-      <c r="I31" s="14">
-        <v>4</v>
-      </c>
-      <c r="J31" s="14">
+      <c r="I31" s="1">
+        <v>4</v>
+      </c>
+      <c r="J31" s="1">
         <v>3</v>
       </c>
       <c r="K31" s="2">
@@ -1541,28 +1535,28 @@
       <c r="B32" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="14" t="s">
+      <c r="C32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="14" t="s">
+      <c r="E32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="14">
-        <v>2</v>
-      </c>
-      <c r="H32" s="14">
+      <c r="G32" s="1">
+        <v>2</v>
+      </c>
+      <c r="H32" s="1">
         <v>8</v>
       </c>
-      <c r="I32" s="14">
-        <v>2</v>
-      </c>
-      <c r="J32" s="14">
+      <c r="I32" s="1">
+        <v>2</v>
+      </c>
+      <c r="J32" s="1">
         <v>2</v>
       </c>
       <c r="K32" s="2">
@@ -1572,28 +1566,28 @@
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="14" t="s">
+      <c r="C33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F33" s="14" t="s">
+      <c r="E33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="1">
         <v>8</v>
       </c>
-      <c r="H33" s="14">
+      <c r="H33" s="1">
         <v>7</v>
       </c>
-      <c r="I33" s="14">
-        <v>2</v>
-      </c>
-      <c r="J33" s="14">
+      <c r="I33" s="1">
+        <v>2</v>
+      </c>
+      <c r="J33" s="1">
         <v>3</v>
       </c>
       <c r="K33" s="2">
@@ -1603,14 +1597,14 @@
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -1620,28 +1614,28 @@
       <c r="B35" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" s="14" t="s">
+      <c r="C35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G35" s="14">
-        <v>4</v>
-      </c>
-      <c r="H35" s="14">
+      <c r="G35" s="1">
+        <v>4</v>
+      </c>
+      <c r="H35" s="1">
         <v>6</v>
       </c>
-      <c r="I35" s="14">
-        <v>2</v>
-      </c>
-      <c r="J35" s="14">
+      <c r="I35" s="1">
+        <v>2</v>
+      </c>
+      <c r="J35" s="1">
         <v>2</v>
       </c>
       <c r="K35" s="2">
@@ -1651,28 +1645,28 @@
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="14" t="s">
+      <c r="C36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="1">
         <v>32</v>
       </c>
-      <c r="H36" s="14">
-        <v>4</v>
-      </c>
-      <c r="I36" s="14">
-        <v>1</v>
-      </c>
-      <c r="J36" s="14">
+      <c r="H36" s="1">
+        <v>4</v>
+      </c>
+      <c r="I36" s="1">
+        <v>1</v>
+      </c>
+      <c r="J36" s="1">
         <v>2</v>
       </c>
       <c r="K36" s="2">
@@ -1684,28 +1678,28 @@
       <c r="B37" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="14" t="s">
+      <c r="C37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="14">
-        <v>2</v>
-      </c>
-      <c r="H37" s="14">
+      <c r="G37" s="1">
+        <v>2</v>
+      </c>
+      <c r="H37" s="1">
         <v>5</v>
       </c>
-      <c r="I37" s="14">
-        <v>2</v>
-      </c>
-      <c r="J37" s="14">
+      <c r="I37" s="1">
+        <v>2</v>
+      </c>
+      <c r="J37" s="1">
         <v>1</v>
       </c>
       <c r="K37" s="2">
@@ -1715,28 +1709,28 @@
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="14" t="s">
+      <c r="C38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G38" s="1">
         <v>8</v>
       </c>
-      <c r="H38" s="14">
+      <c r="H38" s="1">
         <v>5</v>
       </c>
-      <c r="I38" s="14">
-        <v>1</v>
-      </c>
-      <c r="J38" s="14">
+      <c r="I38" s="1">
+        <v>1</v>
+      </c>
+      <c r="J38" s="1">
         <v>2</v>
       </c>
       <c r="K38" s="2">
@@ -1746,14 +1740,13 @@
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -1763,28 +1756,28 @@
       <c r="B40" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="14" t="s">
+      <c r="C40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F40" s="14">
-        <v>1</v>
-      </c>
-      <c r="G40" s="14">
-        <v>1</v>
-      </c>
-      <c r="H40" s="14">
+      <c r="E40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
+      <c r="H40" s="1">
         <v>6</v>
       </c>
-      <c r="I40" s="14">
+      <c r="I40" s="1">
         <v>3</v>
       </c>
-      <c r="J40" s="14">
+      <c r="J40" s="1">
         <v>1</v>
       </c>
       <c r="K40" s="2">
@@ -1794,28 +1787,28 @@
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" s="14" t="s">
+      <c r="C41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="E41" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G41" s="14">
-        <v>4</v>
-      </c>
-      <c r="H41" s="14">
+      <c r="G41" s="1">
+        <v>4</v>
+      </c>
+      <c r="H41" s="1">
         <v>6</v>
       </c>
-      <c r="I41" s="14">
-        <v>2</v>
-      </c>
-      <c r="J41" s="14">
+      <c r="I41" s="1">
+        <v>2</v>
+      </c>
+      <c r="J41" s="1">
         <v>2</v>
       </c>
       <c r="K41" s="2">
@@ -1827,28 +1820,28 @@
       <c r="B42" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="14" t="s">
+      <c r="C42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G42" s="14">
-        <v>2</v>
-      </c>
-      <c r="H42" s="14">
+      <c r="G42" s="1">
+        <v>2</v>
+      </c>
+      <c r="H42" s="1">
         <v>9</v>
       </c>
-      <c r="I42" s="14">
+      <c r="I42" s="1">
         <v>3</v>
       </c>
-      <c r="J42" s="14">
+      <c r="J42" s="1">
         <v>2</v>
       </c>
       <c r="K42" s="2">
@@ -1927,14 +1920,14 @@
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
       <c r="M46" s="2"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -1944,76 +1937,165 @@
       <c r="B47" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="2"/>
+      <c r="C47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="1">
+        <v>2</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I47" s="1">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1">
+        <v>4</v>
+      </c>
+      <c r="K47" s="1">
+        <v>1</v>
+      </c>
+      <c r="L47" s="1">
+        <v>1</v>
+      </c>
+      <c r="M47" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="2"/>
+      <c r="C48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" s="1">
+        <v>2</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J48" s="1">
+        <v>4</v>
+      </c>
+      <c r="K48" s="1">
+        <v>2</v>
+      </c>
+      <c r="L48" s="1">
+        <v>1</v>
+      </c>
+      <c r="M48" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="2"/>
+      <c r="C49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H49" s="1">
+        <v>4</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J49" s="1">
+        <v>5</v>
+      </c>
+      <c r="K49" s="1">
+        <v>1</v>
+      </c>
+      <c r="L49" s="1">
+        <v>2</v>
+      </c>
+      <c r="M49" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="2"/>
+      <c r="C50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H50" s="1">
+        <v>2</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J50" s="1">
+        <v>5</v>
+      </c>
+      <c r="K50" s="1">
+        <v>1</v>
+      </c>
+      <c r="L50" s="1">
+        <v>2</v>
+      </c>
+      <c r="M50" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="7"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
       <c r="M51" s="2"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -2023,31 +2105,35 @@
       <c r="B52" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
+      <c r="C52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
       <c r="M52" s="2"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
+      <c r="C53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
       <c r="M53" s="2"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -2055,16 +2141,18 @@
       <c r="B54" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
+      <c r="C54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
       <c r="M54" s="2"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
finished polynomial kernel, started exponential
</commit_message>
<xml_diff>
--- a/results/knn-ald_iris/Iris.xlsx
+++ b/results/knn-ald_iris/Iris.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\MLTool_matlab\results\knn-ald_iris\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MATLAB\MLTool\results\knn-ald_iris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64F444C-BB88-4F7B-AA51-CC53B775891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AD96C3-BE96-4670-A299-39113A1B2A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALD" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="58">
   <si>
     <t>4 attributes</t>
   </si>
@@ -190,6 +190,18 @@
   </si>
   <si>
     <t>0.8</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>0.0020</t>
+  </si>
+  <si>
+    <t>EXPONENTIAL KERNEL</t>
+  </si>
+  <si>
+    <t>0.6</t>
   </si>
 </sst>
 </file>
@@ -317,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -351,9 +363,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,20 +644,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -669,7 +678,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -682,7 +691,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>39</v>
       </c>
@@ -713,7 +722,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>30</v>
       </c>
@@ -748,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
       <c r="B5" s="6"/>
       <c r="C5" s="1" t="s">
@@ -780,7 +789,7 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="6" t="s">
         <v>14</v>
@@ -814,7 +823,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
@@ -846,13 +855,13 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="7"/>
       <c r="K8" s="3"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>29</v>
       </c>
@@ -888,7 +897,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
@@ -920,7 +929,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="6" t="s">
         <v>14</v>
@@ -954,7 +963,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="6"/>
       <c r="C12" s="1" t="s">
@@ -986,7 +995,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="6"/>
       <c r="C13" s="1"/>
@@ -1000,7 +1009,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>32</v>
       </c>
@@ -1036,7 +1045,7 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
@@ -1068,7 +1077,7 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="6" t="s">
         <v>14</v>
@@ -1102,7 +1111,7 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
@@ -1134,7 +1143,7 @@
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="7"/>
       <c r="D18" s="1"/>
@@ -1147,7 +1156,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>31</v>
       </c>
@@ -1183,7 +1192,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="6"/>
       <c r="C20" s="1" t="s">
@@ -1215,7 +1224,7 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="6" t="s">
         <v>14</v>
@@ -1249,7 +1258,7 @@
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8"/>
       <c r="B22" s="12"/>
       <c r="C22" s="4" t="s">
@@ -1281,7 +1290,7 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1294,7 +1303,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>41</v>
       </c>
@@ -1326,7 +1335,7 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>30</v>
       </c>
@@ -1361,7 +1370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="6"/>
       <c r="C26" s="1" t="s">
@@ -1393,7 +1402,7 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="6" t="s">
         <v>14</v>
@@ -1427,7 +1436,7 @@
       </c>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="6"/>
       <c r="C28" s="1" t="s">
@@ -1459,12 +1468,12 @@
       </c>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="7"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>29</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="6"/>
       <c r="C31" s="1" t="s">
@@ -1530,7 +1539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="6" t="s">
         <v>14</v>
@@ -1563,7 +1572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="6"/>
       <c r="C33" s="1" t="s">
@@ -1594,7 +1603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="B34" s="6"/>
       <c r="C34" s="1"/>
@@ -1607,7 +1616,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>32</v>
       </c>
@@ -1642,7 +1651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="6"/>
       <c r="C36" s="1" t="s">
@@ -1673,7 +1682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="6" t="s">
         <v>14</v>
@@ -1706,7 +1715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="6"/>
       <c r="C38" s="1" t="s">
@@ -1737,7 +1746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="B39" s="7"/>
       <c r="D39" s="1"/>
@@ -1749,7 +1758,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>31</v>
       </c>
@@ -1784,7 +1793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="6"/>
       <c r="C41" s="1" t="s">
@@ -1815,7 +1824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
       <c r="B42" s="6" t="s">
         <v>14</v>
@@ -1848,7 +1857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="8"/>
       <c r="B43" s="12"/>
       <c r="C43" s="4" t="s">
@@ -1879,8 +1888,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
         <v>47</v>
       </c>
@@ -1917,7 +1926,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="B46" s="6"/>
       <c r="C46" s="1"/>
@@ -1930,7 +1939,7 @@
       <c r="L46" s="1"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>32</v>
       </c>
@@ -1952,7 +1961,7 @@
       <c r="G47" s="1">
         <v>2</v>
       </c>
-      <c r="H47" s="14" t="s">
+      <c r="H47" s="1" t="s">
         <v>33</v>
       </c>
       <c r="I47" s="1">
@@ -1971,7 +1980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="13"/>
       <c r="B48" s="6"/>
       <c r="C48" s="1" t="s">
@@ -2008,7 +2017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="B49" s="6" t="s">
         <v>14</v>
@@ -2047,7 +2056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
       <c r="B50" s="6"/>
       <c r="C50" s="1" t="s">
@@ -2084,7 +2093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="13"/>
       <c r="B51" s="7"/>
       <c r="D51" s="1"/>
@@ -2098,7 +2107,7 @@
       <c r="L51" s="1"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
         <v>31</v>
       </c>
@@ -2108,35 +2117,75 @@
       <c r="C52" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="2"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" s="1">
+        <v>8</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J52" s="1">
+        <v>9</v>
+      </c>
+      <c r="K52" s="1">
+        <v>3</v>
+      </c>
+      <c r="L52" s="1">
+        <v>2</v>
+      </c>
+      <c r="M52" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
       <c r="B53" s="6"/>
       <c r="C53" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="2"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="1">
+        <v>4</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H53" s="1">
+        <v>8</v>
+      </c>
+      <c r="I53" s="1">
+        <v>2</v>
+      </c>
+      <c r="J53" s="1">
+        <v>5</v>
+      </c>
+      <c r="K53" s="1">
+        <v>2</v>
+      </c>
+      <c r="L53" s="1">
+        <v>1</v>
+      </c>
+      <c r="M53" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="7"/>
       <c r="B54" s="6" t="s">
         <v>14</v>
@@ -2144,33 +2193,286 @@
       <c r="C54" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="2"/>
-    </row>
-    <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J54" s="1">
+        <v>6</v>
+      </c>
+      <c r="K54" s="1">
+        <v>2</v>
+      </c>
+      <c r="L54" s="1">
+        <v>2</v>
+      </c>
+      <c r="M54" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="8"/>
       <c r="B55" s="12"/>
       <c r="C55" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="5"/>
+      <c r="D55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="4">
+        <v>8</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J55" s="4">
+        <v>6</v>
+      </c>
+      <c r="K55" s="4">
+        <v>2</v>
+      </c>
+      <c r="L55" s="4">
+        <v>2</v>
+      </c>
+      <c r="M55" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="11"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K57" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L57" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M57" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" s="13"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="2"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" s="13"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="2"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A61" s="13"/>
+      <c r="B61" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="2"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A62" s="13"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="2"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A63" s="13"/>
+      <c r="B63" s="7"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="2"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A64" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="2"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A65" s="13"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="2"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A66" s="7"/>
+      <c r="B66" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="2"/>
+    </row>
+    <row r="67" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="8"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2183,7 +2485,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2195,7 +2497,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2209,7 +2511,7 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
finished exponential tests and updated xlsx file
</commit_message>
<xml_diff>
--- a/results/knn-ald_iris/Iris.xlsx
+++ b/results/knn-ald_iris/Iris.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MATLAB\MLTool\results\knn-ald_iris\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\MLTool_matlab\results\knn-ald_iris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AD96C3-BE96-4670-A299-39113A1B2A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B77C26-852C-4558-B221-0A69446CAF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALD" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="61">
   <si>
     <t>4 attributes</t>
   </si>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>0.6</t>
+  </si>
+  <si>
+    <t>86.67</t>
+  </si>
+  <si>
+    <t>83.81</t>
+  </si>
+  <si>
+    <t>CAUCHY KERNEL</t>
   </si>
 </sst>
 </file>
@@ -329,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,6 +372,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,20 +656,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M67"/>
+  <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71:M79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -678,7 +690,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -691,7 +703,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>39</v>
       </c>
@@ -722,7 +734,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>30</v>
       </c>
@@ -757,7 +769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="6"/>
       <c r="C5" s="1" t="s">
@@ -789,7 +801,7 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="6" t="s">
         <v>14</v>
@@ -823,7 +835,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
@@ -855,13 +867,13 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="7"/>
       <c r="K8" s="3"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>29</v>
       </c>
@@ -897,7 +909,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
@@ -929,7 +941,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="6" t="s">
         <v>14</v>
@@ -963,7 +975,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="6"/>
       <c r="C12" s="1" t="s">
@@ -995,7 +1007,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="6"/>
       <c r="C13" s="1"/>
@@ -1009,7 +1021,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>32</v>
       </c>
@@ -1045,7 +1057,7 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
@@ -1077,7 +1089,7 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="6" t="s">
         <v>14</v>
@@ -1111,7 +1123,7 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
@@ -1143,7 +1155,7 @@
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="7"/>
       <c r="D18" s="1"/>
@@ -1156,7 +1168,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>31</v>
       </c>
@@ -1192,7 +1204,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="6"/>
       <c r="C20" s="1" t="s">
@@ -1224,7 +1236,7 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="6" t="s">
         <v>14</v>
@@ -1258,7 +1270,7 @@
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="12"/>
       <c r="C22" s="4" t="s">
@@ -1290,7 +1302,7 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1303,7 +1315,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>41</v>
       </c>
@@ -1335,7 +1347,7 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>30</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="6"/>
       <c r="C26" s="1" t="s">
@@ -1402,7 +1414,7 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="6" t="s">
         <v>14</v>
@@ -1436,7 +1448,7 @@
       </c>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="6"/>
       <c r="C28" s="1" t="s">
@@ -1468,12 +1480,12 @@
       </c>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="7"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>29</v>
       </c>
@@ -1508,7 +1520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="6"/>
       <c r="C31" s="1" t="s">
@@ -1539,7 +1551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="6" t="s">
         <v>14</v>
@@ -1572,7 +1584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="6"/>
       <c r="C33" s="1" t="s">
@@ -1603,7 +1615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="6"/>
       <c r="C34" s="1"/>
@@ -1616,7 +1628,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>32</v>
       </c>
@@ -1651,7 +1663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="6"/>
       <c r="C36" s="1" t="s">
@@ -1682,7 +1694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="6" t="s">
         <v>14</v>
@@ -1715,7 +1727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="6"/>
       <c r="C38" s="1" t="s">
@@ -1746,7 +1758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="7"/>
       <c r="D39" s="1"/>
@@ -1758,7 +1770,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>31</v>
       </c>
@@ -1793,7 +1805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="6"/>
       <c r="C41" s="1" t="s">
@@ -1824,7 +1836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="6" t="s">
         <v>14</v>
@@ -1857,7 +1869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
       <c r="B43" s="12"/>
       <c r="C43" s="4" t="s">
@@ -1888,8 +1900,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>47</v>
       </c>
@@ -1926,7 +1938,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="6"/>
       <c r="C46" s="1"/>
@@ -1939,7 +1951,7 @@
       <c r="L46" s="1"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>32</v>
       </c>
@@ -1980,7 +1992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="6"/>
       <c r="C48" s="1" t="s">
@@ -2017,7 +2029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="6" t="s">
         <v>14</v>
@@ -2056,7 +2068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="6"/>
       <c r="C50" s="1" t="s">
@@ -2093,7 +2105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="7"/>
       <c r="D51" s="1"/>
@@ -2107,7 +2119,7 @@
       <c r="L51" s="1"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>31</v>
       </c>
@@ -2148,7 +2160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="6"/>
       <c r="C53" s="1" t="s">
@@ -2185,7 +2197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="6" t="s">
         <v>14</v>
@@ -2224,7 +2236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8"/>
       <c r="B55" s="12"/>
       <c r="C55" s="4" t="s">
@@ -2261,8 +2273,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="57" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>56</v>
       </c>
@@ -2278,28 +2290,22 @@
         <v>21</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="J57" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K57" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L57" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M57" s="10" t="s">
+      <c r="K57" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="6"/>
       <c r="C58" s="1"/>
@@ -2307,12 +2313,12 @@
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="2"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K58" s="2"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>32</v>
       </c>
@@ -2322,35 +2328,63 @@
       <c r="C59" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="2"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D59" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" s="1">
+        <v>4</v>
+      </c>
+      <c r="I59" s="1">
+        <v>1</v>
+      </c>
+      <c r="J59" s="1">
+        <v>1</v>
+      </c>
+      <c r="K59" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="6"/>
       <c r="C60" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="2"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D60" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G60" s="1">
+        <v>32</v>
+      </c>
+      <c r="H60" s="1">
+        <v>7</v>
+      </c>
+      <c r="I60" s="1">
+        <v>2</v>
+      </c>
+      <c r="J60" s="1">
+        <v>2</v>
+      </c>
+      <c r="K60" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="6" t="s">
         <v>14</v>
@@ -2358,35 +2392,63 @@
       <c r="C61" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="2"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D61" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" s="1">
+        <v>64</v>
+      </c>
+      <c r="H61" s="1">
+        <v>7</v>
+      </c>
+      <c r="I61" s="1">
+        <v>2</v>
+      </c>
+      <c r="J61" s="1">
+        <v>2</v>
+      </c>
+      <c r="K61" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="6"/>
       <c r="C62" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="2"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G62" s="1">
+        <v>64</v>
+      </c>
+      <c r="H62" s="1">
+        <v>4</v>
+      </c>
+      <c r="I62" s="1">
+        <v>1</v>
+      </c>
+      <c r="J62" s="1">
+        <v>1</v>
+      </c>
+      <c r="K62" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="7"/>
       <c r="D63" s="1"/>
@@ -2396,11 +2458,9 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="2"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K63" s="2"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>31</v>
       </c>
@@ -2410,35 +2470,63 @@
       <c r="C64" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="2"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D64" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G64" s="1">
+        <v>64</v>
+      </c>
+      <c r="H64" s="1">
+        <v>5</v>
+      </c>
+      <c r="I64" s="1">
+        <v>2</v>
+      </c>
+      <c r="J64" s="1">
+        <v>1</v>
+      </c>
+      <c r="K64" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="6"/>
       <c r="C65" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="2"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D65" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H65" s="1">
+        <v>8</v>
+      </c>
+      <c r="I65" s="1">
+        <v>3</v>
+      </c>
+      <c r="J65" s="1">
+        <v>2</v>
+      </c>
+      <c r="K65" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="6" t="s">
         <v>14</v>
@@ -2446,36 +2534,278 @@
       <c r="C66" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="2"/>
-    </row>
-    <row r="67" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D66" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66" s="1">
+        <v>4</v>
+      </c>
+      <c r="H66" s="1">
+        <v>19</v>
+      </c>
+      <c r="I66" s="1">
+        <v>5</v>
+      </c>
+      <c r="J66" s="1">
+        <v>4</v>
+      </c>
+      <c r="K66" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
       <c r="B67" s="12"/>
       <c r="C67" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-      <c r="M67" s="5"/>
+      <c r="D67" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" s="4">
+        <v>1</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H67" s="4">
+        <v>6</v>
+      </c>
+      <c r="I67" s="4">
+        <v>2</v>
+      </c>
+      <c r="J67" s="4">
+        <v>2</v>
+      </c>
+      <c r="K67" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B69" s="11"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J69" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K69" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L69" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M69" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="2"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="2"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="2"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="13"/>
+      <c r="B73" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="2"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="13"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="2"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="13"/>
+      <c r="B75" s="7"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="2"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="2"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="13"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="2"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="7"/>
+      <c r="B78" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="2"/>
+    </row>
+    <row r="79" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="8"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2485,7 +2815,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2497,7 +2827,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2511,7 +2841,7 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
finished tests with spok ald iris log kernel
</commit_message>
<xml_diff>
--- a/results/knn-ald_iris/Iris.xlsx
+++ b/results/knn-ald_iris/Iris.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\MLTool_matlab\results\knn-ald_iris\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MLTool_matlab\results\knn-ald_iris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B77C26-852C-4558-B221-0A69446CAF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9BA67C-A25D-4D37-8532-301FE55D3F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALD" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="65">
   <si>
     <t>4 attributes</t>
   </si>
@@ -211,6 +211,18 @@
   </si>
   <si>
     <t>CAUCHY KERNEL</t>
+  </si>
+  <si>
+    <t>89.52</t>
+  </si>
+  <si>
+    <t>LOG KERNEL</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+  <si>
+    <t>2.2</t>
   </si>
 </sst>
 </file>
@@ -338,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,9 +384,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M79"/>
+  <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71:M79"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2359,7 +2368,7 @@
       <c r="C60" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D60" s="14" t="s">
+      <c r="D60" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E60" s="1" t="s">
@@ -2495,7 +2504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="6"/>
       <c r="C65" s="1" t="s">
@@ -2526,7 +2535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="6" t="s">
         <v>14</v>
@@ -2559,7 +2568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
       <c r="B67" s="12"/>
       <c r="C67" s="4" t="s">
@@ -2590,8 +2599,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
         <v>60</v>
       </c>
@@ -2607,28 +2616,22 @@
         <v>21</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I69" s="9" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K69" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L69" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M69" s="10" t="s">
+      <c r="K69" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
       <c r="B70" s="6"/>
       <c r="C70" s="1"/>
@@ -2636,12 +2639,12 @@
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
       <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="2"/>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K70" s="2"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>32</v>
       </c>
@@ -2651,35 +2654,63 @@
       <c r="C71" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="2"/>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D71" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F71" s="1">
+        <v>1</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H71" s="1">
+        <v>4</v>
+      </c>
+      <c r="I71" s="1">
+        <v>1</v>
+      </c>
+      <c r="J71" s="1">
+        <v>1</v>
+      </c>
+      <c r="K71" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
       <c r="B72" s="6"/>
       <c r="C72" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="2"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D72" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G72" s="1">
+        <v>8</v>
+      </c>
+      <c r="H72" s="1">
+        <v>4</v>
+      </c>
+      <c r="I72" s="1">
+        <v>1</v>
+      </c>
+      <c r="J72" s="1">
+        <v>1</v>
+      </c>
+      <c r="K72" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="6" t="s">
         <v>14</v>
@@ -2687,35 +2718,63 @@
       <c r="C73" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="2"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D73" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G73" s="1">
+        <v>8</v>
+      </c>
+      <c r="H73" s="1">
+        <v>7</v>
+      </c>
+      <c r="I73" s="1">
+        <v>2</v>
+      </c>
+      <c r="J73" s="1">
+        <v>2</v>
+      </c>
+      <c r="K73" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
       <c r="B74" s="6"/>
       <c r="C74" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="2"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D74" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G74" s="1">
+        <v>32</v>
+      </c>
+      <c r="H74" s="1">
+        <v>5</v>
+      </c>
+      <c r="I74" s="1">
+        <v>1</v>
+      </c>
+      <c r="J74" s="1">
+        <v>2</v>
+      </c>
+      <c r="K74" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
       <c r="B75" s="7"/>
       <c r="D75" s="1"/>
@@ -2725,11 +2784,9 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
-      <c r="M75" s="2"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K75" s="2"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>31</v>
       </c>
@@ -2739,35 +2796,63 @@
       <c r="C76" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
-      <c r="M76" s="2"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D76" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76" s="1">
+        <v>8</v>
+      </c>
+      <c r="H76" s="1">
+        <v>6</v>
+      </c>
+      <c r="I76" s="1">
+        <v>2</v>
+      </c>
+      <c r="J76" s="1">
+        <v>1</v>
+      </c>
+      <c r="K76" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="13"/>
       <c r="B77" s="6"/>
       <c r="C77" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="2"/>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D77" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G77" s="1">
+        <v>16</v>
+      </c>
+      <c r="H77" s="1">
+        <v>7</v>
+      </c>
+      <c r="I77" s="1">
+        <v>2</v>
+      </c>
+      <c r="J77" s="1">
+        <v>2</v>
+      </c>
+      <c r="K77" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="6" t="s">
         <v>14</v>
@@ -2775,33 +2860,406 @@
       <c r="C78" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-      <c r="K78" s="1"/>
-      <c r="L78" s="1"/>
-      <c r="M78" s="2"/>
-    </row>
-    <row r="79" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D78" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G78" s="1">
+        <v>8</v>
+      </c>
+      <c r="H78" s="1">
+        <v>10</v>
+      </c>
+      <c r="I78" s="1">
+        <v>2</v>
+      </c>
+      <c r="J78" s="1">
+        <v>3</v>
+      </c>
+      <c r="K78" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="8"/>
       <c r="B79" s="12"/>
       <c r="C79" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="4"/>
-      <c r="K79" s="4"/>
-      <c r="L79" s="4"/>
-      <c r="M79" s="5"/>
+      <c r="D79" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G79" s="4">
+        <v>16</v>
+      </c>
+      <c r="H79" s="4">
+        <v>8</v>
+      </c>
+      <c r="I79" s="4">
+        <v>2</v>
+      </c>
+      <c r="J79" s="4">
+        <v>2</v>
+      </c>
+      <c r="K79" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B81" s="11"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H81" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I81" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J81" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K81" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L81" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="13"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="2"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F83" s="1">
+        <v>-128</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H83" s="1">
+        <v>3</v>
+      </c>
+      <c r="I83" s="1">
+        <v>39</v>
+      </c>
+      <c r="J83" s="1">
+        <v>10</v>
+      </c>
+      <c r="K83" s="1">
+        <v>14</v>
+      </c>
+      <c r="L83" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="13"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F84" s="1">
+        <v>-16</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I84" s="1">
+        <v>31</v>
+      </c>
+      <c r="J84" s="1">
+        <v>29</v>
+      </c>
+      <c r="K84" s="1">
+        <v>1</v>
+      </c>
+      <c r="L84" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="13"/>
+      <c r="B85" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="1">
+        <v>-512</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H85" s="1">
+        <v>3</v>
+      </c>
+      <c r="I85" s="1">
+        <v>26</v>
+      </c>
+      <c r="J85" s="1">
+        <v>10</v>
+      </c>
+      <c r="K85" s="1">
+        <v>9</v>
+      </c>
+      <c r="L85" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="13"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F86" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I86" s="1">
+        <v>27</v>
+      </c>
+      <c r="J86" s="1">
+        <v>1</v>
+      </c>
+      <c r="K86" s="1">
+        <v>1</v>
+      </c>
+      <c r="L86" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="13"/>
+      <c r="B87" s="7"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="2"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F88" s="1">
+        <v>-4</v>
+      </c>
+      <c r="G88" s="1">
+        <v>1</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I88" s="1">
+        <v>47</v>
+      </c>
+      <c r="J88" s="1">
+        <v>20</v>
+      </c>
+      <c r="K88" s="1">
+        <v>14</v>
+      </c>
+      <c r="L88" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="13"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F89" s="1">
+        <v>-8</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H89" s="1">
+        <v>3</v>
+      </c>
+      <c r="I89" s="1">
+        <v>34</v>
+      </c>
+      <c r="J89" s="1">
+        <v>32</v>
+      </c>
+      <c r="K89" s="1">
+        <v>1</v>
+      </c>
+      <c r="L89" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="7"/>
+      <c r="B90" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F90" s="1">
+        <v>-256</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H90" s="1">
+        <v>3</v>
+      </c>
+      <c r="I90" s="1">
+        <v>45</v>
+      </c>
+      <c r="J90" s="1">
+        <v>15</v>
+      </c>
+      <c r="K90" s="1">
+        <v>17</v>
+      </c>
+      <c r="L90" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="8"/>
+      <c r="B91" s="12"/>
+      <c r="C91" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F91" s="4">
+        <v>-32</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I91" s="4">
+        <v>33</v>
+      </c>
+      <c r="J91" s="4">
+        <v>31</v>
+      </c>
+      <c r="K91" s="4">
+        <v>1</v>
+      </c>
+      <c r="L91" s="5">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished iris knn ald tests with all kernels
</commit_message>
<xml_diff>
--- a/results/knn-ald_iris/Iris.xlsx
+++ b/results/knn-ald_iris/Iris.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MLTool_matlab\results\knn-ald_iris\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MATLAB\MLTool\results\knn-ald_iris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9BA67C-A25D-4D37-8532-301FE55D3F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B70EB2-67A7-427F-9565-468EE8A23F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALD" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="69">
   <si>
     <t>4 attributes</t>
   </si>
@@ -223,12 +223,27 @@
   </si>
   <si>
     <t>2.2</t>
+  </si>
+  <si>
+    <t>SIGMOID KERNEL</t>
+  </si>
+  <si>
+    <t>KMOD KERNEL</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>92.83</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -350,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -384,6 +399,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,20 +683,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M91"/>
+  <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="L115" sqref="L115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -699,7 +717,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -712,7 +730,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>39</v>
       </c>
@@ -743,7 +761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>30</v>
       </c>
@@ -778,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
       <c r="B5" s="6"/>
       <c r="C5" s="1" t="s">
@@ -810,7 +828,7 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="6" t="s">
         <v>14</v>
@@ -844,7 +862,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
@@ -876,13 +894,13 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="7"/>
       <c r="K8" s="3"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>29</v>
       </c>
@@ -918,7 +936,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
@@ -950,7 +968,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="6" t="s">
         <v>14</v>
@@ -984,7 +1002,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="6"/>
       <c r="C12" s="1" t="s">
@@ -1016,7 +1034,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="6"/>
       <c r="C13" s="1"/>
@@ -1030,7 +1048,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>32</v>
       </c>
@@ -1066,7 +1084,7 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
@@ -1098,7 +1116,7 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="6" t="s">
         <v>14</v>
@@ -1132,7 +1150,7 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
@@ -1164,7 +1182,7 @@
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="7"/>
       <c r="D18" s="1"/>
@@ -1177,7 +1195,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>31</v>
       </c>
@@ -1213,7 +1231,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="6"/>
       <c r="C20" s="1" t="s">
@@ -1245,7 +1263,7 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="6" t="s">
         <v>14</v>
@@ -1279,7 +1297,7 @@
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8"/>
       <c r="B22" s="12"/>
       <c r="C22" s="4" t="s">
@@ -1311,7 +1329,7 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1324,7 +1342,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>41</v>
       </c>
@@ -1356,7 +1374,7 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>30</v>
       </c>
@@ -1391,7 +1409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="6"/>
       <c r="C26" s="1" t="s">
@@ -1423,7 +1441,7 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="6" t="s">
         <v>14</v>
@@ -1457,7 +1475,7 @@
       </c>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="6"/>
       <c r="C28" s="1" t="s">
@@ -1489,12 +1507,12 @@
       </c>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="7"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>29</v>
       </c>
@@ -1529,7 +1547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="6"/>
       <c r="C31" s="1" t="s">
@@ -1560,7 +1578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="6" t="s">
         <v>14</v>
@@ -1593,7 +1611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="6"/>
       <c r="C33" s="1" t="s">
@@ -1624,7 +1642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="B34" s="6"/>
       <c r="C34" s="1"/>
@@ -1637,7 +1655,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>32</v>
       </c>
@@ -1672,7 +1690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="6"/>
       <c r="C36" s="1" t="s">
@@ -1703,7 +1721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="6" t="s">
         <v>14</v>
@@ -1736,7 +1754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="6"/>
       <c r="C38" s="1" t="s">
@@ -1767,7 +1785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="B39" s="7"/>
       <c r="D39" s="1"/>
@@ -1779,7 +1797,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>31</v>
       </c>
@@ -1814,7 +1832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="6"/>
       <c r="C41" s="1" t="s">
@@ -1845,7 +1863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
       <c r="B42" s="6" t="s">
         <v>14</v>
@@ -1878,7 +1896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="8"/>
       <c r="B43" s="12"/>
       <c r="C43" s="4" t="s">
@@ -1909,8 +1927,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
         <v>47</v>
       </c>
@@ -1947,7 +1965,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="B46" s="6"/>
       <c r="C46" s="1"/>
@@ -1960,7 +1978,7 @@
       <c r="L46" s="1"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>32</v>
       </c>
@@ -2001,7 +2019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="13"/>
       <c r="B48" s="6"/>
       <c r="C48" s="1" t="s">
@@ -2038,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="B49" s="6" t="s">
         <v>14</v>
@@ -2077,7 +2095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
       <c r="B50" s="6"/>
       <c r="C50" s="1" t="s">
@@ -2114,7 +2132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="13"/>
       <c r="B51" s="7"/>
       <c r="D51" s="1"/>
@@ -2128,7 +2146,7 @@
       <c r="L51" s="1"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
         <v>31</v>
       </c>
@@ -2169,7 +2187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
       <c r="B53" s="6"/>
       <c r="C53" s="1" t="s">
@@ -2206,7 +2224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="7"/>
       <c r="B54" s="6" t="s">
         <v>14</v>
@@ -2245,7 +2263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="8"/>
       <c r="B55" s="12"/>
       <c r="C55" s="4" t="s">
@@ -2282,8 +2300,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="11" t="s">
         <v>56</v>
       </c>
@@ -2314,7 +2332,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="13"/>
       <c r="B58" s="6"/>
       <c r="C58" s="1"/>
@@ -2327,7 +2345,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
         <v>32</v>
       </c>
@@ -2362,7 +2380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="13"/>
       <c r="B60" s="6"/>
       <c r="C60" s="1" t="s">
@@ -2393,7 +2411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="13"/>
       <c r="B61" s="6" t="s">
         <v>14</v>
@@ -2426,7 +2444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="13"/>
       <c r="B62" s="6"/>
       <c r="C62" s="1" t="s">
@@ -2457,7 +2475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="13"/>
       <c r="B63" s="7"/>
       <c r="D63" s="1"/>
@@ -2469,7 +2487,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
         <v>31</v>
       </c>
@@ -2504,7 +2522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="13"/>
       <c r="B65" s="6"/>
       <c r="C65" s="1" t="s">
@@ -2535,7 +2553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="7"/>
       <c r="B66" s="6" t="s">
         <v>14</v>
@@ -2568,7 +2586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="8"/>
       <c r="B67" s="12"/>
       <c r="C67" s="4" t="s">
@@ -2599,8 +2617,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="69" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="11" t="s">
         <v>60</v>
       </c>
@@ -2631,7 +2649,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="13"/>
       <c r="B70" s="6"/>
       <c r="C70" s="1"/>
@@ -2644,7 +2662,7 @@
       <c r="J70" s="1"/>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
         <v>32</v>
       </c>
@@ -2679,7 +2697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="13"/>
       <c r="B72" s="6"/>
       <c r="C72" s="1" t="s">
@@ -2710,7 +2728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="13"/>
       <c r="B73" s="6" t="s">
         <v>14</v>
@@ -2743,7 +2761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="13"/>
       <c r="B74" s="6"/>
       <c r="C74" s="1" t="s">
@@ -2774,7 +2792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="13"/>
       <c r="B75" s="7"/>
       <c r="D75" s="1"/>
@@ -2786,7 +2804,7 @@
       <c r="J75" s="1"/>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
         <v>31</v>
       </c>
@@ -2821,7 +2839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="13"/>
       <c r="B77" s="6"/>
       <c r="C77" s="1" t="s">
@@ -2852,7 +2870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="7"/>
       <c r="B78" s="6" t="s">
         <v>14</v>
@@ -2885,7 +2903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="8"/>
       <c r="B79" s="12"/>
       <c r="C79" s="4" t="s">
@@ -2916,8 +2934,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="81" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="81" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="11" t="s">
         <v>62</v>
       </c>
@@ -2951,7 +2969,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="13"/>
       <c r="B82" s="6"/>
       <c r="C82" s="1"/>
@@ -2964,7 +2982,7 @@
       <c r="K82" s="1"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="13" t="s">
         <v>32</v>
       </c>
@@ -3002,7 +3020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="13"/>
       <c r="B84" s="6"/>
       <c r="C84" s="1" t="s">
@@ -3036,7 +3054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="13"/>
       <c r="B85" s="6" t="s">
         <v>14</v>
@@ -3072,7 +3090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="13"/>
       <c r="B86" s="6"/>
       <c r="C86" s="1" t="s">
@@ -3106,7 +3124,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="13"/>
       <c r="B87" s="7"/>
       <c r="D87" s="1"/>
@@ -3119,7 +3137,7 @@
       <c r="K87" s="1"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
         <v>31</v>
       </c>
@@ -3157,7 +3175,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="13"/>
       <c r="B89" s="6"/>
       <c r="C89" s="1" t="s">
@@ -3191,7 +3209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="7"/>
       <c r="B90" s="6" t="s">
         <v>14</v>
@@ -3227,7 +3245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="8"/>
       <c r="B91" s="12"/>
       <c r="C91" s="4" t="s">
@@ -3259,6 +3277,697 @@
       </c>
       <c r="L91" s="5">
         <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="93" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B93" s="11"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G93" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H93" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I93" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J93" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K93" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L93" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A94" s="13"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="2"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A95" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I95" s="1">
+        <v>6</v>
+      </c>
+      <c r="J95" s="1">
+        <v>2</v>
+      </c>
+      <c r="K95" s="1">
+        <v>1</v>
+      </c>
+      <c r="L95" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A96" s="13"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I96" s="1">
+        <v>7</v>
+      </c>
+      <c r="J96" s="1">
+        <v>2</v>
+      </c>
+      <c r="K96" s="1">
+        <v>3</v>
+      </c>
+      <c r="L96" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A97" s="13"/>
+      <c r="B97" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" s="1">
+        <v>96.19</v>
+      </c>
+      <c r="E97" s="1">
+        <v>100</v>
+      </c>
+      <c r="F97" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="G97" s="1">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="H97" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="I97" s="1">
+        <v>7</v>
+      </c>
+      <c r="J97" s="1">
+        <v>3</v>
+      </c>
+      <c r="K97" s="1">
+        <v>2</v>
+      </c>
+      <c r="L97" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A98" s="13"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" s="1">
+        <v>90.48</v>
+      </c>
+      <c r="E98" s="1">
+        <v>93.33</v>
+      </c>
+      <c r="F98" s="1">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="G98" s="1">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="H98" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="I98" s="1">
+        <v>6</v>
+      </c>
+      <c r="J98" s="1">
+        <v>2</v>
+      </c>
+      <c r="K98" s="1">
+        <v>2</v>
+      </c>
+      <c r="L98" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A99" s="13"/>
+      <c r="B99" s="7"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="2"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A100" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D100" s="1">
+        <v>94.29</v>
+      </c>
+      <c r="E100" s="1">
+        <v>93.33</v>
+      </c>
+      <c r="F100" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="G100" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="H100" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I100" s="1">
+        <v>5</v>
+      </c>
+      <c r="J100" s="1">
+        <v>1</v>
+      </c>
+      <c r="K100" s="1">
+        <v>3</v>
+      </c>
+      <c r="L100" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A101" s="13"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" s="1">
+        <v>93.33</v>
+      </c>
+      <c r="E101" s="1">
+        <v>91.11</v>
+      </c>
+      <c r="F101" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G101" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H101" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="I101" s="1">
+        <v>6</v>
+      </c>
+      <c r="J101" s="1">
+        <v>2</v>
+      </c>
+      <c r="K101" s="1">
+        <v>2</v>
+      </c>
+      <c r="L101" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A102" s="7"/>
+      <c r="B102" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D102" s="1">
+        <v>94.29</v>
+      </c>
+      <c r="E102" s="1">
+        <v>93.33</v>
+      </c>
+      <c r="F102" s="1">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="G102" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="H102" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I102" s="1">
+        <v>6</v>
+      </c>
+      <c r="J102" s="1">
+        <v>1</v>
+      </c>
+      <c r="K102" s="1">
+        <v>3</v>
+      </c>
+      <c r="L102" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="8"/>
+      <c r="B103" s="12"/>
+      <c r="C103" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D103" s="4">
+        <v>88.57</v>
+      </c>
+      <c r="E103" s="4">
+        <v>91.11</v>
+      </c>
+      <c r="F103" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G103" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H103" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="I103" s="4">
+        <v>7</v>
+      </c>
+      <c r="J103" s="4">
+        <v>2</v>
+      </c>
+      <c r="K103" s="4">
+        <v>2</v>
+      </c>
+      <c r="L103" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="105" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B105" s="11"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G105" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H105" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I105" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J105" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K105" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L105" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A106" s="13"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+      <c r="L106" s="2"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A107" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G107" s="1">
+        <v>64</v>
+      </c>
+      <c r="H107" s="1">
+        <v>8</v>
+      </c>
+      <c r="I107" s="1">
+        <v>7</v>
+      </c>
+      <c r="J107" s="1">
+        <v>2</v>
+      </c>
+      <c r="K107" s="1">
+        <v>2</v>
+      </c>
+      <c r="L107" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A108" s="13"/>
+      <c r="B108" s="6"/>
+      <c r="C108" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" s="1">
+        <v>93.33</v>
+      </c>
+      <c r="E108" s="1">
+        <v>95.56</v>
+      </c>
+      <c r="F108" s="1">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="G108" s="1">
+        <v>32</v>
+      </c>
+      <c r="H108" s="1">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="I108" s="1">
+        <v>5</v>
+      </c>
+      <c r="J108" s="1">
+        <v>2</v>
+      </c>
+      <c r="K108" s="1">
+        <v>1</v>
+      </c>
+      <c r="L108" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A109" s="13"/>
+      <c r="B109" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D109" s="1">
+        <v>90.48</v>
+      </c>
+      <c r="E109" s="1">
+        <v>95.56</v>
+      </c>
+      <c r="F109" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="G109" s="1">
+        <v>4</v>
+      </c>
+      <c r="H109" s="1">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="I109" s="1">
+        <v>7</v>
+      </c>
+      <c r="J109" s="1">
+        <v>2</v>
+      </c>
+      <c r="K109" s="1">
+        <v>2</v>
+      </c>
+      <c r="L109" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A110" s="13"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" s="1">
+        <v>97.14</v>
+      </c>
+      <c r="E110" s="1">
+        <v>95.56</v>
+      </c>
+      <c r="F110" s="1">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="G110" s="1">
+        <v>16</v>
+      </c>
+      <c r="H110" s="1">
+        <v>32</v>
+      </c>
+      <c r="I110" s="1">
+        <v>7</v>
+      </c>
+      <c r="J110" s="1">
+        <v>2</v>
+      </c>
+      <c r="K110" s="1">
+        <v>2</v>
+      </c>
+      <c r="L110" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A111" s="13"/>
+      <c r="B111" s="7"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+      <c r="L111" s="2"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A112" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D112" s="1">
+        <v>94.29</v>
+      </c>
+      <c r="E112" s="1">
+        <v>95.56</v>
+      </c>
+      <c r="F112" s="1">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="G112" s="1">
+        <v>16</v>
+      </c>
+      <c r="H112" s="1">
+        <v>64</v>
+      </c>
+      <c r="I112" s="1">
+        <v>6</v>
+      </c>
+      <c r="J112" s="1">
+        <v>2</v>
+      </c>
+      <c r="K112" s="1">
+        <v>1</v>
+      </c>
+      <c r="L112" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A113" s="13"/>
+      <c r="B113" s="6"/>
+      <c r="C113" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D113" s="1">
+        <v>92.38</v>
+      </c>
+      <c r="E113" s="1">
+        <v>97.78</v>
+      </c>
+      <c r="F113" s="1">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="G113" s="1">
+        <v>64</v>
+      </c>
+      <c r="H113" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="I113" s="1">
+        <v>4</v>
+      </c>
+      <c r="J113" s="1">
+        <v>1</v>
+      </c>
+      <c r="K113" s="1">
+        <v>1</v>
+      </c>
+      <c r="L113" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A114" s="7"/>
+      <c r="B114" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D114" s="1">
+        <v>92.38</v>
+      </c>
+      <c r="E114" s="1">
+        <v>93.33</v>
+      </c>
+      <c r="F114" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="G114" s="1">
+        <v>32</v>
+      </c>
+      <c r="H114" s="1">
+        <v>16</v>
+      </c>
+      <c r="I114" s="1">
+        <v>11</v>
+      </c>
+      <c r="J114" s="1">
+        <v>4</v>
+      </c>
+      <c r="K114" s="1">
+        <v>3</v>
+      </c>
+      <c r="L114" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="8"/>
+      <c r="B115" s="12"/>
+      <c r="C115" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D115" s="4">
+        <v>92.38</v>
+      </c>
+      <c r="E115" s="4">
+        <v>95.56</v>
+      </c>
+      <c r="F115" s="4">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="G115" s="4">
+        <v>16</v>
+      </c>
+      <c r="H115" s="4">
+        <v>32</v>
+      </c>
+      <c r="I115" s="4">
+        <v>8</v>
+      </c>
+      <c r="J115" s="4">
+        <v>3</v>
+      </c>
+      <c r="K115" s="4">
+        <v>2</v>
+      </c>
+      <c r="L115" s="5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3273,7 +3982,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -3285,7 +3994,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -3299,7 +4008,7 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>